<commit_message>
Add, Edit, Delete job
</commit_message>
<xml_diff>
--- a/Commusoft-Stage2&Live/TestDatas/Datasheet.xlsx
+++ b/Commusoft-Stage2&Live/TestDatas/Datasheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f0c4ada4d22ca239/Desktop/Automation/Commusoft--Stage-Live/Commusoft-Stage2^0Live/TestDatas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Commusoft--Stage-Live\Commusoft--Stage-Live\Commusoft-Stage2&amp;Live\TestDatas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_C8B71A78C72DFF6E272D0D83D79E4249CF1E396B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85BCAE77-0341-432B-903D-EF0569743874}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE3F599-78FE-4B5A-B3BD-53B601D1D4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -150,10 +150,10 @@
     <t>To create and accept an estimate without parts been added with retension and intial payment.</t>
   </si>
   <si>
-    <t>demo123</t>
-  </si>
-  <si>
-    <t>azar</t>
+    <t>nirai</t>
+  </si>
+  <si>
+    <t>nirai123</t>
   </si>
 </sst>
 </file>
@@ -539,7 +539,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -561,7 +561,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -569,7 +569,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Prefinal and final invoices with all breakdowns
</commit_message>
<xml_diff>
--- a/Commusoft-Stage2&Live/TestDatas/Datasheet.xlsx
+++ b/Commusoft-Stage2&Live/TestDatas/Datasheet.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f0c4ada4d22ca239/Desktop/Automation/Commusoft--Stage-Live/Commusoft-Stage2^0Live/TestDatas/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{4462ECC3-86FD-4788-9E60-D383FCC806F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2472" windowWidth="12876" windowHeight="3516"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -12,7 +18,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -145,17 +150,17 @@
     <t>To create and accept an estimate without parts been added with retension and intial payment.</t>
   </si>
   <si>
-    <t>karna</t>
-  </si>
-  <si>
     <t>demo123</t>
+  </si>
+  <si>
+    <t>azar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,7 +258,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -285,9 +290,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -319,6 +342,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -494,20 +535,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -515,23 +556,23 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -539,7 +580,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -554,21 +595,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
     <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="88.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -591,7 +632,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -602,7 +643,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>18</v>
       </c>
@@ -610,7 +651,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>20</v>
       </c>
@@ -618,7 +659,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>22</v>
       </c>
@@ -626,7 +667,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>24</v>
       </c>
@@ -634,7 +675,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>26</v>
       </c>
@@ -642,7 +683,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>27</v>
       </c>
@@ -650,7 +691,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>29</v>
       </c>
@@ -658,7 +699,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>31</v>
       </c>
@@ -666,7 +707,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>33</v>
       </c>
@@ -674,7 +715,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>35</v>
       </c>
@@ -682,7 +723,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>37</v>
       </c>
@@ -690,7 +731,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>39</v>
       </c>
@@ -704,12 +745,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Recall and abort job
</commit_message>
<xml_diff>
--- a/Commusoft-Stage2&Live/TestDatas/Datasheet.xlsx
+++ b/Commusoft-Stage2&Live/TestDatas/Datasheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f0c4ada4d22ca239/Desktop/Automation/Commusoft--Stage-Live/Commusoft-Stage2^0Live/TestDatas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Commusoft--Stage-Live\Commusoft--Stage-Live\Commusoft-Stage2&amp;Live\TestDatas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{4462ECC3-86FD-4788-9E60-D383FCC806F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284D4AB7-FBFE-4447-9E0B-B76A316003D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -153,7 +153,7 @@
     <t>demo123</t>
   </si>
   <si>
-    <t>azar</t>
+    <t>ezhil</t>
   </si>
 </sst>
 </file>
@@ -539,7 +539,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
external address as invoice address
</commit_message>
<xml_diff>
--- a/Commusoft-Stage2&Live/TestDatas/Datasheet.xlsx
+++ b/Commusoft-Stage2&Live/TestDatas/Datasheet.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f0c4ada4d22ca239/Desktop/Commusoft/Commusoft--Stage-Live/Commusoft-Stage2^0Live/TestDatas/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_676DC69220667B4E712D0D83D79E42493F1EBF3F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52525AA2-7384-4850-BF0A-08865E43B026}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2472" windowWidth="12876" windowHeight="3516"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -12,7 +18,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -148,14 +153,14 @@
     <t>demo123</t>
   </si>
   <si>
-    <t>karna</t>
+    <t>azar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,7 +258,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -285,9 +290,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -319,6 +342,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -494,20 +535,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -515,7 +556,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -523,7 +564,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -531,7 +572,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -539,7 +580,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -554,21 +595,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
     <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="88.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -591,7 +632,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -602,7 +643,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>18</v>
       </c>
@@ -610,7 +651,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>20</v>
       </c>
@@ -618,7 +659,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>22</v>
       </c>
@@ -626,7 +667,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>24</v>
       </c>
@@ -634,7 +675,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>26</v>
       </c>
@@ -642,7 +683,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>27</v>
       </c>
@@ -650,7 +691,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>29</v>
       </c>
@@ -658,7 +699,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>31</v>
       </c>
@@ -666,7 +707,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>33</v>
       </c>
@@ -674,7 +715,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>35</v>
       </c>
@@ -682,7 +723,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>37</v>
       </c>
@@ -690,7 +731,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>39</v>
       </c>
@@ -704,12 +745,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add,edit & delete the job on diary
</commit_message>
<xml_diff>
--- a/Commusoft-Stage2&Live/TestDatas/Datasheet.xlsx
+++ b/Commusoft-Stage2&Live/TestDatas/Datasheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f0c4ada4d22ca239/Desktop/Commusoft/Commusoft--Stage-Live/Commusoft-Stage2^0Live/TestDatas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Commusoft--Stage-Live\Commusoft-Stage2&amp;Live\TestDatas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_676DC69220667B4E712D0D83D79E42493F1EBF3F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52525AA2-7384-4850-BF0A-08865E43B026}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E179BC3-85BF-4812-BAF9-4FE433646ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -153,7 +153,7 @@
     <t>demo123</t>
   </si>
   <si>
-    <t>azar</t>
+    <t>ezhil</t>
   </si>
 </sst>
 </file>
@@ -539,7 +539,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updated few changes on smoke test
</commit_message>
<xml_diff>
--- a/Commusoft-Stage2&Live/TestDatas/Datasheet.xlsx
+++ b/Commusoft-Stage2&Live/TestDatas/Datasheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Commusoft--Stage-Live\Commusoft-Stage2&amp;Live\TestDatas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f0c4ada4d22ca239/Desktop/Commusoft/Commusoft--Stage-Live/Commusoft-Stage2^0Live/TestDatas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E179BC3-85BF-4812-BAF9-4FE433646ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{9E179BC3-85BF-4812-BAF9-4FE433646ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63289533-C32A-4147-9E32-53F4F5386049}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -153,7 +153,7 @@
     <t>demo123</t>
   </si>
   <si>
-    <t>ezhil</t>
+    <t>azar</t>
   </si>
 </sst>
 </file>
@@ -539,7 +539,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Estimate (Reject estimate,Multiple option & Option clone estimate)
</commit_message>
<xml_diff>
--- a/Commusoft-Stage2&Live/TestDatas/Datasheet.xlsx
+++ b/Commusoft-Stage2&Live/TestDatas/Datasheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f0c4ada4d22ca239/Desktop/Commusoft/Commusoft--Stage-Live/Commusoft-Stage2^0Live/TestDatas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Commusoft--Stage-Live\Commusoft-Stage2&amp;Live\TestDatas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{9E179BC3-85BF-4812-BAF9-4FE433646ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63289533-C32A-4147-9E32-53F4F5386049}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E515B6-C4E7-4849-A6E8-602421660167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -153,7 +153,7 @@
     <t>demo123</t>
   </si>
   <si>
-    <t>azar</t>
+    <t>ezhil</t>
   </si>
 </sst>
 </file>
@@ -539,7 +539,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
QA-138 & updated few invoice testcases to smoke test
</commit_message>
<xml_diff>
--- a/Commusoft-Stage2&Live/TestDatas/Datasheet.xlsx
+++ b/Commusoft-Stage2&Live/TestDatas/Datasheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Commusoft--Stage-Live\Commusoft-Stage2&amp;Live\TestDatas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f0c4ada4d22ca239/Desktop/Commusoft/Commusoft--Stage-Live/Commusoft-Stage2^0Live/TestDatas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA3D65C-530B-4A12-B4B3-E0AF733B99C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{CEA3D65C-530B-4A12-B4B3-E0AF733B99C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA51F904-BCD2-44D2-8822-5BF438EA6C51}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -153,7 +153,7 @@
     <t>demo123</t>
   </si>
   <si>
-    <t>ezhil</t>
+    <t>azar</t>
   </si>
 </sst>
 </file>
@@ -539,7 +539,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>